<commit_message>
Updated disease and threshold dictionaries
Updated disease and threshold dictionaries
</commit_message>
<xml_diff>
--- a/inst/extdata/disease_dictionary.xlsx
+++ b/inst/extdata/disease_dictionary.xlsx
@@ -1,25 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Spina\Desktop\WHO_AFRO\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldhealthorg-my.sharepoint.com/personal/moussanaf_who_int/Documents/Documents/GitHub/epichecks/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_399C71DCFC6B7C82A3C7A0E2E886952F692DD682" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{93C7C6FA-EA6A-4D7E-AF02-2724221D7F61}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$A$1:$B$123</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="157">
   <si>
     <t>Acute Watery Diarrhea</t>
   </si>
@@ -397,9 +401,6 @@
   </si>
   <si>
     <t>Acute and Chronic Viral Hepatitis</t>
-  </si>
-  <si>
-    <t>Acute Haemorrhagic Fever Syndrome</t>
   </si>
   <si>
     <t>Marburg</t>
@@ -498,7 +499,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -841,21 +842,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B117" sqref="B117"/>
+      <selection activeCell="A124" sqref="A124"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="50" customWidth="1"/>
-    <col min="4" max="4" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>112</v>
       </c>
@@ -865,7 +866,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -874,25 +875,25 @@
       </c>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>152</v>
-      </c>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>131</v>
-      </c>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -900,7 +901,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -908,7 +909,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -916,15 +917,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -932,15 +933,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -948,7 +949,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -956,7 +957,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -964,7 +965,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>116</v>
       </c>
@@ -972,7 +973,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -980,7 +981,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -988,15 +989,15 @@
         <v>117</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -1004,7 +1005,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -1013,7 +1014,7 @@
       </c>
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -1021,7 +1022,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -1029,7 +1030,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -1037,7 +1038,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -1045,7 +1046,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>118</v>
       </c>
@@ -1053,7 +1054,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>119</v>
       </c>
@@ -1061,7 +1062,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -1069,7 +1070,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>20</v>
       </c>
@@ -1077,7 +1078,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>21</v>
       </c>
@@ -1085,7 +1086,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -1093,7 +1094,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>23</v>
       </c>
@@ -1102,7 +1103,7 @@
       </c>
       <c r="C30" s="3"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>24</v>
       </c>
@@ -1111,31 +1112,31 @@
       </c>
       <c r="C31" s="3"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>25</v>
       </c>
       <c r="B32" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>26</v>
       </c>
       <c r="B33" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>27</v>
       </c>
       <c r="B34" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>28</v>
       </c>
@@ -1143,23 +1144,23 @@
         <v>121</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>29</v>
       </c>
       <c r="B36" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>30</v>
       </c>
       <c r="B37" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>31</v>
       </c>
@@ -1168,7 +1169,7 @@
       </c>
       <c r="C38" s="3"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>32</v>
       </c>
@@ -1177,7 +1178,7 @@
       </c>
       <c r="C39" s="3"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>33</v>
       </c>
@@ -1185,15 +1186,15 @@
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>34</v>
       </c>
       <c r="B41" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>35</v>
       </c>
@@ -1201,7 +1202,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>36</v>
       </c>
@@ -1209,7 +1210,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>37</v>
       </c>
@@ -1217,7 +1218,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>38</v>
       </c>
@@ -1225,7 +1226,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>39</v>
       </c>
@@ -1233,7 +1234,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>40</v>
       </c>
@@ -1241,15 +1242,15 @@
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>41</v>
       </c>
       <c r="B48" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>42</v>
       </c>
@@ -1257,7 +1258,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>43</v>
       </c>
@@ -1265,23 +1266,23 @@
         <v>43</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>44</v>
       </c>
       <c r="B51" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>45</v>
       </c>
       <c r="B52" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>46</v>
       </c>
@@ -1289,7 +1290,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>47</v>
       </c>
@@ -1298,7 +1299,7 @@
       </c>
       <c r="C54" s="3"/>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>48</v>
       </c>
@@ -1307,7 +1308,7 @@
       </c>
       <c r="C55" s="3"/>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>49</v>
       </c>
@@ -1315,7 +1316,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>50</v>
       </c>
@@ -1323,7 +1324,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>51</v>
       </c>
@@ -1331,7 +1332,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>52</v>
       </c>
@@ -1339,7 +1340,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>53</v>
       </c>
@@ -1347,7 +1348,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>54</v>
       </c>
@@ -1355,15 +1356,15 @@
         <v>54</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>55</v>
       </c>
       <c r="B62" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>56</v>
       </c>
@@ -1371,7 +1372,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>57</v>
       </c>
@@ -1379,7 +1380,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>58</v>
       </c>
@@ -1387,7 +1388,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>59</v>
       </c>
@@ -1395,7 +1396,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>60</v>
       </c>
@@ -1403,7 +1404,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>61</v>
       </c>
@@ -1411,31 +1412,31 @@
         <v>57</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>62</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
+        <v>126</v>
+      </c>
+      <c r="B70" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
         <v>127</v>
       </c>
-      <c r="B70" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>128</v>
-      </c>
       <c r="B71" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>63</v>
       </c>
@@ -1443,7 +1444,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>64</v>
       </c>
@@ -1451,7 +1452,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>65</v>
       </c>
@@ -1459,7 +1460,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>66</v>
       </c>
@@ -1467,7 +1468,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>67</v>
       </c>
@@ -1475,7 +1476,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>68</v>
       </c>
@@ -1483,15 +1484,15 @@
         <v>68</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>69</v>
       </c>
       <c r="B78" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>70</v>
       </c>
@@ -1499,7 +1500,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>71</v>
       </c>
@@ -1507,7 +1508,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>72</v>
       </c>
@@ -1516,15 +1517,15 @@
       </c>
       <c r="C81" s="3"/>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>73</v>
       </c>
       <c r="B82" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>74</v>
       </c>
@@ -1532,7 +1533,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>75</v>
       </c>
@@ -1540,64 +1541,64 @@
         <v>110</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B85" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>76</v>
       </c>
       <c r="B86" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>77</v>
       </c>
       <c r="B87" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>134</v>
-      </c>
       <c r="B88" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>78</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C89" s="3"/>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>79</v>
       </c>
       <c r="B90" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>80</v>
       </c>
       <c r="B91" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>81</v>
       </c>
@@ -1605,7 +1606,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>82</v>
       </c>
@@ -1613,7 +1614,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>83</v>
       </c>
@@ -1622,7 +1623,7 @@
       </c>
       <c r="C94" s="3"/>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>84</v>
       </c>
@@ -1630,7 +1631,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>85</v>
       </c>
@@ -1638,31 +1639,31 @@
         <v>85</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>86</v>
       </c>
       <c r="B97" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>87</v>
       </c>
       <c r="B98" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>134</v>
+      </c>
+      <c r="B99" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>135</v>
-      </c>
-      <c r="B99" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>88</v>
       </c>
@@ -1671,7 +1672,7 @@
       </c>
       <c r="C100" s="3"/>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>89</v>
       </c>
@@ -1679,7 +1680,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>90</v>
       </c>
@@ -1687,7 +1688,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>111</v>
       </c>
@@ -1695,7 +1696,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>91</v>
       </c>
@@ -1703,15 +1704,15 @@
         <v>91</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>92</v>
       </c>
       <c r="B105" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>93</v>
       </c>
@@ -1719,7 +1720,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>94</v>
       </c>
@@ -1727,7 +1728,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>95</v>
       </c>
@@ -1736,7 +1737,7 @@
       </c>
       <c r="C108" s="3"/>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>96</v>
       </c>
@@ -1744,7 +1745,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>97</v>
       </c>
@@ -1752,7 +1753,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>98</v>
       </c>
@@ -1760,7 +1761,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>99</v>
       </c>
@@ -1768,7 +1769,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>100</v>
       </c>
@@ -1776,15 +1777,15 @@
         <v>100</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>101</v>
       </c>
       <c r="B114" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>102</v>
       </c>
@@ -1792,7 +1793,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>103</v>
       </c>
@@ -1801,42 +1802,42 @@
       </c>
       <c r="C116" s="3"/>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>104</v>
       </c>
-      <c r="B117" s="3" t="s">
-        <v>126</v>
+      <c r="B117" t="s">
+        <v>104</v>
       </c>
       <c r="C117" s="3"/>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
+        <v>138</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C118" s="3"/>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
         <v>139</v>
       </c>
-      <c r="B118" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="C118" s="3"/>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>140</v>
-      </c>
       <c r="B119" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C119" s="3"/>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>105</v>
       </c>
       <c r="B120" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>106</v>
       </c>
@@ -1844,7 +1845,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>107</v>
       </c>
@@ -1852,17 +1853,18 @@
         <v>107</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>108</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C123" s="3"/>
       <c r="D123" s="3"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B123" xr:uid="{E33A55BC-5053-4FA2-AF55-EF9BCD86C250}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>

<commit_message>
Disease and threshold dictionaries
</commit_message>
<xml_diff>
--- a/inst/extdata/disease_dictionary.xlsx
+++ b/inst/extdata/disease_dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldhealthorg-my.sharepoint.com/personal/moussanaf_who_int/Documents/Documents/GitHub/epichecks/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_399C71DCFC6B7C82A3C7A0E2E886952F692DD682" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{93C7C6FA-EA6A-4D7E-AF02-2724221D7F61}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="11_399C71DCFC6B7C82A3C7A0E2E886952F692DD682" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C2D488C0-4949-4023-85B6-87C74539EB29}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,18 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$A$1:$B$123</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -846,7 +857,7 @@
   <dimension ref="A1:D123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A124" sqref="A124"/>
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1522,7 +1533,7 @@
         <v>73</v>
       </c>
       <c r="B82" t="s">
-        <v>131</v>
+        <v>73</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>